<commit_message>
added the new 2021 data
</commit_message>
<xml_diff>
--- a/app/2021_input_data.xlsx
+++ b/app/2021_input_data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data_science\colaberry\MIT_Solve_dashboard\notebooks\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data_science\colaberry\MIT_Solve_dashboard\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1B4544-1731-4F92-801B-89BDEF38A83F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C4E6CB-8F70-4387-B7E4-34F2FDB6AC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{E3D59B11-78D3-4466-9D47-CC32E0038EB3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Partner Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Solver Team Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Solver Team Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Partner Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2542,10 +2542,13 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:X1048576"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -5184,7 +5187,7 @@
   <dimension ref="A1:AU117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AZ1048576"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>